<commit_message>
first working draft of Tools->Import Model Data
</commit_message>
<xml_diff>
--- a/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
+++ b/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14664" windowHeight="5904" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14664" windowHeight="5904" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -155,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
   <si>
     <t>AMRW</t>
   </si>
@@ -254,9 +254,6 @@
   </si>
   <si>
     <t>Path</t>
-  </si>
-  <si>
-    <t>Site</t>
   </si>
   <si>
     <t>Prefix</t>
@@ -678,7 +675,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -693,9 +690,7 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -706,13 +701,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>58</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>24</v>
@@ -942,26 +937,27 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -977,9 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -991,19 +985,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
       </c>
       <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1011,13 +1005,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE(B2,C2,"-",A2,"-",D2)</f>
@@ -1029,13 +1023,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E16" si="0">CONCATENATE(B3,C3,"-",A3,"-",D3)</f>
@@ -1047,13 +1041,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -1065,13 +1059,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -1083,13 +1077,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -1101,13 +1095,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1119,13 +1113,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -1137,13 +1131,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -1155,13 +1149,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -1173,13 +1167,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -1191,13 +1185,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -1209,13 +1203,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -1227,13 +1221,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -1245,13 +1239,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -1263,13 +1257,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
model-output storage for multiple scenarios (instead of linking to models)  this is a followup on work by @tjrocha
</commit_message>
<xml_diff>
--- a/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
+++ b/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14664" windowHeight="5904" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14664" windowHeight="5904" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
     <sheet name="SiteMapping" sheetId="1" r:id="rId2"/>
     <sheet name="ScenarioMapping" sheetId="3" r:id="rId3"/>
     <sheet name="1" sheetId="2" r:id="rId4"/>
-    <sheet name="2" sheetId="5" r:id="rId5"/>
+    <sheet name="2" sheetId="7" r:id="rId5"/>
     <sheet name="3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -154,8 +154,42 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>JCuhaciyan</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>JCuhaciyan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I propose that the number of columns in these individual scenario sheets can vary (depending on the complexity of the directory structure), but that there will always be a column named "FilePath" that contains the full path name for each input file.  </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="64">
   <si>
     <t>AMRW</t>
   </si>
@@ -332,6 +366,21 @@
   </si>
   <si>
     <t>SiteName</t>
+  </si>
+  <si>
+    <t>TimeInterval</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>cfs</t>
+  </si>
+  <si>
+    <t>Scenario2</t>
   </si>
 </sst>
 </file>
@@ -934,10 +983,10 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,20 +996,37 @@
     <col min="3" max="3" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2">
         <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -971,9 +1037,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -983,7 +1051,7 @@
     <col min="5" max="5" width="192.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>56</v>
       </c>
@@ -999,8 +1067,11 @@
       <c r="E1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1017,8 +1088,11 @@
         <f>CONCATENATE(B2,C2,"-",A2,"-",D2)</f>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1035,8 +1109,11 @@
         <f t="shared" ref="E3:E16" si="0">CONCATENATE(B3,C3,"-",A3,"-",D3)</f>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P2-AUGW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1053,8 +1130,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P3-BUM-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1071,8 +1151,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P4-CLE-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1089,8 +1172,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P5-CLFW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1107,8 +1193,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P6-EASW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1125,8 +1214,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P7-KAC-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1143,8 +1235,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P8-KEE-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1161,8 +1256,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P9-KIOW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1179,8 +1277,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P10-NACW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1197,8 +1298,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P11-PARW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1215,8 +1319,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P12-RIM-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1233,8 +1340,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P13-UMTW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1251,8 +1361,11 @@
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P14-YGVW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1268,6 +1381,9 @@
       <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P15-YUMW-biascorrected_streamflow-provisional_0.1.csv</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1277,16 +1393,344 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="27.109375" customWidth="1"/>
+    <col min="5" max="5" width="192.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>63</v>
+      </c>
+      <c r="F15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
working example with two scenarios ref #57
</commit_message>
<xml_diff>
--- a/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
+++ b/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KTarbet\Documents\project\pisces\PiscesTestData\data\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\PN6200\Studies\RMJOC-II Climate Change Study\Modeling\Deschutes_MonthlyMODSIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="65">
   <si>
     <t>AMRW</t>
   </si>
@@ -308,48 +308,6 @@
     <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/</t>
   </si>
   <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P2</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P3</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P4</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P5</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P6</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P7</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P8</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P9</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P10</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P11</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P12</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P13</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P14</t>
-  </si>
-  <si>
-    <t>CCSM4_RCP45_BCSD_VIC_P15</t>
-  </si>
-  <si>
     <t>ScenarioName</t>
   </si>
   <si>
@@ -381,6 +339,51 @@
   </si>
   <si>
     <t>Scenario2</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.1.csv</t>
+  </si>
+  <si>
+    <t>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.1.csv</t>
   </si>
 </sst>
 </file>
@@ -724,7 +727,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -750,13 +753,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>24</v>
@@ -998,13 +1001,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1015,18 +1018,18 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1039,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1053,7 +1056,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -1068,7 +1071,7 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1089,7 +1092,7 @@
         <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1100,17 +1103,17 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E16" si="0">CONCATENATE(B3,C3,"-",A3,"-",D3)</f>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P2-AUGW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1121,17 +1124,17 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P3-BUM-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1142,17 +1145,17 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P4-CLE-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1163,17 +1166,17 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P5-CLFW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1184,17 +1187,17 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>37</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P6-EASW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1205,17 +1208,17 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P7-KAC-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1226,17 +1229,17 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>37</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P8-KEE-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1247,17 +1250,17 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P9-KIOW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1268,17 +1271,17 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>37</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P10-NACW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1289,17 +1292,17 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P11-PARW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,17 +1313,17 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P12-RIM-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1331,17 +1334,17 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>37</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P13-UMTW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1352,17 +1355,17 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P14-YGVW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1373,17 +1376,17 @@
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P15-YUMW-biascorrected_streamflow-provisional_0.1.csv</v>
+        <v>T:/PN6200/Studies/RMJOC-II Climate Change Study/Data/UW/VIC-UW/CCSM4_RCP45-streamflow-provisional_0.1/Bias_correction/CCSM4_RCP45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.1.csv</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1410,7 +1413,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>32</v>
@@ -1425,7 +1428,7 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1442,10 +1445,10 @@
         <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1456,16 +1459,16 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1476,16 +1479,16 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1496,16 +1499,16 @@
         <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1516,16 +1519,16 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1536,16 +1539,16 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1556,16 +1559,16 @@
         <v>38</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
         <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1576,16 +1579,16 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1596,16 +1599,16 @@
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
         <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1616,16 +1619,16 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1636,16 +1639,16 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1656,16 +1659,16 @@
         <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1676,16 +1679,16 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1696,7 +1699,7 @@
         <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
@@ -1705,7 +1708,7 @@
         <v>63</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1716,16 +1719,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated GCM names in config file
</commit_message>
<xml_diff>
--- a/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
+++ b/PiscesTestData/data/Scenarios/InputScenarioConfig.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" firstSheet="2" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" firstSheet="1" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="UserGuide" sheetId="4" r:id="rId1"/>
@@ -1083,52 +1083,52 @@
     <t>CCSM4_rcp85</t>
   </si>
   <si>
-    <t>CNRMCM5_rcp45</t>
-  </si>
-  <si>
-    <t>CNRMCM5_rcp85</t>
-  </si>
-  <si>
-    <t>CSIROMk360_rcp45</t>
-  </si>
-  <si>
-    <t>CSIROMk360_rcp85</t>
-  </si>
-  <si>
-    <t>GFDLESM2M_rcp45</t>
-  </si>
-  <si>
-    <t>GFDLESM2M_rcp85</t>
-  </si>
-  <si>
-    <t>HadGEM2CC_rcp45</t>
-  </si>
-  <si>
-    <t>HadGEM2CC_rcp85</t>
-  </si>
-  <si>
-    <t>HadGEM2ES_rcp45</t>
-  </si>
-  <si>
-    <t>HadGEM2ES_rcp85</t>
-  </si>
-  <si>
     <t>inmcm4_rcp45</t>
   </si>
   <si>
     <t>inmcm4_rcp85</t>
   </si>
   <si>
-    <t>IPSLCM5AMR_rcp45</t>
-  </si>
-  <si>
-    <t>IPSLCM5AMR_rcp85</t>
-  </si>
-  <si>
     <t>MIROC5_rcp45</t>
   </si>
   <si>
     <t>MIROC5_rcp85</t>
+  </si>
+  <si>
+    <t>CNRM-CM5_rcp45</t>
+  </si>
+  <si>
+    <t>CNRM-CM5_rcp85</t>
+  </si>
+  <si>
+    <t>CSIRO-Mk3-6-0_rcp45</t>
+  </si>
+  <si>
+    <t>CSIRO-Mk3-6-0_rcp85</t>
+  </si>
+  <si>
+    <t>GFDL-ESM2M_rcp45</t>
+  </si>
+  <si>
+    <t>GFDL-ESM2M_rcp85</t>
+  </si>
+  <si>
+    <t>HadGEM2-CC_rcp45</t>
+  </si>
+  <si>
+    <t>HadGEM2-CC_rcp85</t>
+  </si>
+  <si>
+    <t>HadGEM2-ES_rcp45</t>
+  </si>
+  <si>
+    <t>HadGEM2-ES_rcp85</t>
+  </si>
+  <si>
+    <t>IPSL-CM5A-MR_rcp45</t>
+  </si>
+  <si>
+    <t>IPSL-CM5A-MR_rcp85</t>
   </si>
 </sst>
 </file>
@@ -1560,11 +1560,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -1590,11 +1590,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -1620,11 +1620,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -1650,11 +1650,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -1680,11 +1680,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -1710,11 +1710,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -1740,11 +1740,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -1770,11 +1770,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -1800,11 +1800,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -1830,11 +1830,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -1860,11 +1860,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -1890,11 +1890,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -1920,11 +1920,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -1950,11 +1950,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -1980,11 +1980,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP45-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -2067,11 +2067,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -2097,11 +2097,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -2127,11 +2127,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -2157,11 +2157,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -2187,11 +2187,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -2217,11 +2217,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -2247,11 +2247,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -2277,11 +2277,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -2307,11 +2307,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -2337,11 +2337,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -2367,11 +2367,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -2397,11 +2397,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -2427,11 +2427,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -2457,11 +2457,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -2487,11 +2487,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CSIROMk360_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIROMk360_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CSIROMk360_RCP85-streamflow-provisional_0.2\bias_correction\CSIRO-Mk3-6-0_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -2513,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2574,11 +2574,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -2604,11 +2604,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -2634,11 +2634,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -2664,11 +2664,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -2694,11 +2694,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -2724,11 +2724,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -2754,11 +2754,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -2784,11 +2784,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -2814,11 +2814,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -2844,11 +2844,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -2874,11 +2874,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -2904,11 +2904,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -2934,11 +2934,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -2964,11 +2964,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -2994,11 +2994,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP45-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -3081,11 +3081,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -3111,11 +3111,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -3141,11 +3141,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -3171,11 +3171,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -3201,11 +3201,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -3231,11 +3231,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -3261,11 +3261,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -3291,11 +3291,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -3321,11 +3321,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -3351,11 +3351,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -3381,11 +3381,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -3411,11 +3411,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -3441,11 +3441,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -3471,11 +3471,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -3501,11 +3501,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>GFDLESM2M_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>GFDL-ESM2M_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDLESM2M_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\GFDLESM2M_RCP85-streamflow-provisional_0.2\bias_correction\GFDL-ESM2M_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -3588,11 +3588,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -3618,11 +3618,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -3648,11 +3648,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -3678,11 +3678,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -3708,11 +3708,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -3738,11 +3738,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -3768,11 +3768,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -3798,11 +3798,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -3828,11 +3828,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -3858,11 +3858,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -3888,11 +3888,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -3918,11 +3918,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -3948,11 +3948,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -3978,11 +3978,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -4008,11 +4008,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -4095,11 +4095,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -4125,11 +4125,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -4155,11 +4155,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -4185,11 +4185,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -4215,11 +4215,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -4245,11 +4245,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -4275,11 +4275,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -4305,11 +4305,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -4335,11 +4335,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -4365,11 +4365,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -4395,11 +4395,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -4425,11 +4425,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -4455,11 +4455,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -4485,11 +4485,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -4515,11 +4515,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2CC_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-CC_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2CC_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2CC_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-CC_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -4602,11 +4602,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -4632,11 +4632,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -4662,11 +4662,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -4692,11 +4692,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -4722,11 +4722,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -4752,11 +4752,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -4782,11 +4782,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -4812,11 +4812,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -4842,11 +4842,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -4872,11 +4872,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -4902,11 +4902,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -4932,11 +4932,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -4962,11 +4962,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -4992,11 +4992,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -5022,11 +5022,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP45-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -5109,11 +5109,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -5139,11 +5139,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -5169,11 +5169,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -5199,11 +5199,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -5229,11 +5229,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -5259,11 +5259,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -5289,11 +5289,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -5319,11 +5319,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -5349,11 +5349,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -5379,11 +5379,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -5409,11 +5409,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -5439,11 +5439,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -5469,11 +5469,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -5499,11 +5499,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -5529,11 +5529,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>HadGEM2ES_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>HadGEM2-ES_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2ES_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\HadGEM2ES_RCP85-streamflow-provisional_0.2\bias_correction\HadGEM2-ES_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -7324,7 +7324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -7385,11 +7385,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -7415,11 +7415,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -7445,11 +7445,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -7475,11 +7475,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -7505,11 +7505,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -7535,11 +7535,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -7565,11 +7565,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -7595,11 +7595,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -7625,11 +7625,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -7655,11 +7655,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -7685,11 +7685,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -7715,11 +7715,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -7745,11 +7745,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -7775,11 +7775,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -7805,11 +7805,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP45-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -7892,11 +7892,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -7922,11 +7922,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -7952,11 +7952,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -7982,11 +7982,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -8012,11 +8012,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -8042,11 +8042,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -8072,11 +8072,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -8102,11 +8102,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -8132,11 +8132,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -8162,11 +8162,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -8192,11 +8192,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -8222,11 +8222,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -8252,11 +8252,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -8282,11 +8282,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -8312,11 +8312,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>IPSLCM5AMR_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSLCM5AMR_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\IPSLCM5AMR_RCP85-streamflow-provisional_0.2\bias_correction\IPSL-CM5A-MR_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -9356,7 +9356,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9445,7 +9445,7 @@
         <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>40</v>
@@ -9459,7 +9459,7 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>40</v>
@@ -9473,7 +9473,7 @@
         <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>40</v>
@@ -9487,7 +9487,7 @@
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>40</v>
@@ -9501,7 +9501,7 @@
         <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>40</v>
@@ -9515,7 +9515,7 @@
         <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>40</v>
@@ -9529,7 +9529,7 @@
         <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>40</v>
@@ -9543,7 +9543,7 @@
         <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>40</v>
@@ -9557,7 +9557,7 @@
         <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>40</v>
@@ -9571,7 +9571,7 @@
         <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>40</v>
@@ -9599,7 +9599,7 @@
         <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>40</v>
@@ -9613,7 +9613,7 @@
         <v>59</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>40</v>
@@ -9627,7 +9627,7 @@
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -9641,7 +9641,7 @@
         <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>40</v>
@@ -9655,7 +9655,7 @@
         <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>40</v>
@@ -9669,7 +9669,7 @@
         <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>40</v>
@@ -9685,7 +9685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -11774,11 +11774,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -11804,11 +11804,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -11834,11 +11834,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -11864,11 +11864,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -11894,11 +11894,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -11924,11 +11924,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -11954,11 +11954,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -11984,11 +11984,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -12014,11 +12014,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -12044,11 +12044,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -12074,11 +12074,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -12104,11 +12104,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -12134,11 +12134,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -12164,11 +12164,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -12194,11 +12194,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP45-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp45_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>
@@ -12281,11 +12281,11 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A2,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G2" s="1" t="str">
         <f ca="1">CONCATENATE(E2,F2)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-AMRW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -12311,11 +12311,11 @@
       </c>
       <c r="F3" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A3,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G3" s="1" t="str">
         <f t="shared" ref="G3:G16" ca="1" si="1">CONCATENATE(E3,F3)</f>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-AUGW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H3" t="s">
         <v>42</v>
@@ -12341,11 +12341,11 @@
       </c>
       <c r="F4" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A4,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G4" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-BUM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -12371,11 +12371,11 @@
       </c>
       <c r="F5" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A5,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-CLE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -12401,11 +12401,11 @@
       </c>
       <c r="F6" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A6,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G6" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-CLFW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -12431,11 +12431,11 @@
       </c>
       <c r="F7" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A7,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G7" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-EASW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -12461,11 +12461,11 @@
       </c>
       <c r="F8" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A8,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G8" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-KAC-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -12491,11 +12491,11 @@
       </c>
       <c r="F9" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A9,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-KEE-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -12521,11 +12521,11 @@
       </c>
       <c r="F10" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A10,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-KIOW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
@@ -12551,11 +12551,11 @@
       </c>
       <c r="F11" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A11,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-NACW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
@@ -12581,11 +12581,11 @@
       </c>
       <c r="F12" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A12,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-PARW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
@@ -12611,11 +12611,11 @@
       </c>
       <c r="F13" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A13,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-RIM-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
@@ -12641,11 +12641,11 @@
       </c>
       <c r="F14" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A14,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-UMTW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H14" t="s">
         <v>42</v>
@@ -12671,11 +12671,11 @@
       </c>
       <c r="F15" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A15,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-YGVW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H15" t="s">
         <v>42</v>
@@ -12701,11 +12701,11 @@
       </c>
       <c r="F16" t="str">
         <f ca="1">CONCATENATE(VLOOKUP(VALUE(MID(CELL("filename",$A$1),FIND("]",CELL("filename",$A$1))+1,255)),ScenarioMapping!$A$2:$C$22,3,FALSE),"_BCSD_VIC_P1-",A16,"-","biascorrected_streamflow-provisional_0.2.csv")</f>
-        <v>CNRMCM5_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>CNRM-CM5_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRMCM5_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
+        <v>T:\PN6200\Studies\RMJOC-II Climate Change Study\Data\UW\VIC-UW\streamflow-provisional_0.2\CNRMCM5_RCP85-streamflow-provisional_0.2\bias_correction\CNRM-CM5_rcp85_BCSD_VIC_P1-YUMW-biascorrected_streamflow-provisional_0.2.csv</v>
       </c>
       <c r="H16" t="s">
         <v>42</v>

</xml_diff>